<commit_message>
parse specific sheets in the excel file
</commit_message>
<xml_diff>
--- a/privateData/SampleData.xlsx
+++ b/privateData/SampleData.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamez\Documents\GitHub\ExcelParser\privateData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6EB167-AB5B-43B2-9143-E207AF3B1240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FB1191-6DBB-4EFC-AD61-EF6112B8298C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39015" yWindow="1980" windowWidth="12150" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" r:id="rId1"/>
+    <sheet name="Sale Financials" sheetId="2" r:id="rId2"/>
+    <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="26">
   <si>
     <t>Region</t>
   </si>
@@ -118,7 +120,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -150,6 +152,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,12 +167,80 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -180,7 +256,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -216,6 +292,36 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,9 +651,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="A2:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,6 +1693,2014 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D059215-EEA3-4FCF-9058-D1398FE923FF}">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K32" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12">
+        <v>44202</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="13">
+        <v>95</v>
+      </c>
+      <c r="F1" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G1" s="16">
+        <v>189.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>44219</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="13">
+        <v>50</v>
+      </c>
+      <c r="F2" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G2" s="16">
+        <v>999.49999999999989</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>44236</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="13">
+        <v>36</v>
+      </c>
+      <c r="F3" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G3" s="16">
+        <v>179.64000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>44253</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G4" s="16">
+        <v>539.7299999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>44270</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="13">
+        <v>56</v>
+      </c>
+      <c r="F5" s="15">
+        <v>2.99</v>
+      </c>
+      <c r="G5" s="16">
+        <v>167.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>44287</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="13">
+        <v>60</v>
+      </c>
+      <c r="F6" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G6" s="16">
+        <v>299.40000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>44304</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="13">
+        <v>75</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G7" s="16">
+        <v>149.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>44321</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="13">
+        <v>90</v>
+      </c>
+      <c r="F8" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G8" s="16">
+        <v>449.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>44338</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="13">
+        <v>32</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G9" s="16">
+        <v>63.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>44355</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="13">
+        <v>60</v>
+      </c>
+      <c r="F10" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G10" s="16">
+        <v>539.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>44372</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="13">
+        <v>90</v>
+      </c>
+      <c r="F11" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G11" s="16">
+        <v>449.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>44389</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="13">
+        <v>29</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G12" s="16">
+        <v>57.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>44406</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="13">
+        <v>81</v>
+      </c>
+      <c r="F13" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1619.1899999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>44423</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="13">
+        <v>35</v>
+      </c>
+      <c r="F14" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G14" s="16">
+        <v>174.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>44440</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="13">
+        <v>2</v>
+      </c>
+      <c r="F15" s="15">
+        <v>125</v>
+      </c>
+      <c r="G15" s="16">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>44457</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="13">
+        <v>16</v>
+      </c>
+      <c r="F16" s="15">
+        <v>15.99</v>
+      </c>
+      <c r="G16" s="16">
+        <v>255.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>44474</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="13">
+        <v>28</v>
+      </c>
+      <c r="F17" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G17" s="16">
+        <v>251.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>44491</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="13">
+        <v>64</v>
+      </c>
+      <c r="F18" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G18" s="16">
+        <v>575.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>44508</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="13">
+        <v>15</v>
+      </c>
+      <c r="F19" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G19" s="16">
+        <v>299.84999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>44525</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="13">
+        <v>96</v>
+      </c>
+      <c r="F20" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G20" s="16">
+        <v>479.04</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>44542</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="13">
+        <v>67</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G21" s="16">
+        <v>86.43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>44559</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="13">
+        <v>74</v>
+      </c>
+      <c r="F22" s="15">
+        <v>15.99</v>
+      </c>
+      <c r="G22" s="16">
+        <v>1183.26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>44576</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="13">
+        <v>46</v>
+      </c>
+      <c r="F23" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G23" s="16">
+        <v>413.54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>44593</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="13">
+        <v>87</v>
+      </c>
+      <c r="F24" s="15">
+        <v>15</v>
+      </c>
+      <c r="G24" s="16">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>44610</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="13">
+        <v>4</v>
+      </c>
+      <c r="F25" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G25" s="16">
+        <v>19.96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>44627</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="13">
+        <v>7</v>
+      </c>
+      <c r="F26" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G26" s="16">
+        <v>139.92999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>44644</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="13">
+        <v>50</v>
+      </c>
+      <c r="F27" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G27" s="16">
+        <v>249.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
+        <v>44661</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="13">
+        <v>66</v>
+      </c>
+      <c r="F28" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G28" s="16">
+        <v>131.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>44678</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="13">
+        <v>96</v>
+      </c>
+      <c r="F29" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G29" s="16">
+        <v>479.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>44695</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="13">
+        <v>53</v>
+      </c>
+      <c r="F30" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G30" s="16">
+        <v>68.37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>44712</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="13">
+        <v>80</v>
+      </c>
+      <c r="F31" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G31" s="16">
+        <v>719.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>44729</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="13">
+        <v>5</v>
+      </c>
+      <c r="F32" s="15">
+        <v>125</v>
+      </c>
+      <c r="G32" s="16">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>44746</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="13">
+        <v>62</v>
+      </c>
+      <c r="F33" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G33" s="16">
+        <v>309.38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
+        <v>44763</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="13">
+        <v>55</v>
+      </c>
+      <c r="F34" s="15">
+        <v>12.49</v>
+      </c>
+      <c r="G34" s="16">
+        <v>686.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>44780</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="13">
+        <v>42</v>
+      </c>
+      <c r="F35" s="15">
+        <v>23.95</v>
+      </c>
+      <c r="G35" s="16">
+        <v>1005.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>44797</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="13">
+        <v>3</v>
+      </c>
+      <c r="F36" s="15">
+        <v>275</v>
+      </c>
+      <c r="G36" s="16">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
+        <v>44814</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="13">
+        <v>7</v>
+      </c>
+      <c r="F37" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G37" s="16">
+        <v>9.0300000000000011</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>44831</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="13">
+        <v>76</v>
+      </c>
+      <c r="F38" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G38" s="16">
+        <v>151.24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>44848</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="13">
+        <v>57</v>
+      </c>
+      <c r="F39" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G39" s="16">
+        <v>1139.4299999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
+        <v>44865</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="13">
+        <v>14</v>
+      </c>
+      <c r="F40" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G40" s="16">
+        <v>18.060000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>44882</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="13">
+        <v>11</v>
+      </c>
+      <c r="F41" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G41" s="16">
+        <v>54.89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <v>44899</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="13">
+        <v>94</v>
+      </c>
+      <c r="F42" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G42" s="16">
+        <v>1879.06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>44916</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="18">
+        <v>28</v>
+      </c>
+      <c r="F43" s="20">
+        <v>4.99</v>
+      </c>
+      <c r="G43" s="21">
+        <v>139.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CC9D76-EC1A-4E27-A242-FC057F9BC964}">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12">
+        <v>44202</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="13">
+        <v>95</v>
+      </c>
+      <c r="F1" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G1" s="16">
+        <v>189.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>44219</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="13">
+        <v>50</v>
+      </c>
+      <c r="F2" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G2" s="16">
+        <v>999.49999999999989</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>44236</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="13">
+        <v>36</v>
+      </c>
+      <c r="F3" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G3" s="16">
+        <v>179.64000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>44253</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13">
+        <v>27</v>
+      </c>
+      <c r="F4" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G4" s="16">
+        <v>539.7299999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>44270</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="13">
+        <v>56</v>
+      </c>
+      <c r="F5" s="15">
+        <v>2.99</v>
+      </c>
+      <c r="G5" s="16">
+        <v>167.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>44287</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="13">
+        <v>60</v>
+      </c>
+      <c r="F6" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G6" s="16">
+        <v>299.40000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>44304</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="13">
+        <v>75</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G7" s="16">
+        <v>149.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>44321</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="13">
+        <v>90</v>
+      </c>
+      <c r="F8" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G8" s="16">
+        <v>449.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>44338</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="13">
+        <v>32</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G9" s="16">
+        <v>63.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>44355</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="13">
+        <v>60</v>
+      </c>
+      <c r="F10" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G10" s="16">
+        <v>539.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>44372</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="13">
+        <v>90</v>
+      </c>
+      <c r="F11" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G11" s="16">
+        <v>449.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>44389</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="13">
+        <v>29</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G12" s="16">
+        <v>57.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>44406</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="13">
+        <v>81</v>
+      </c>
+      <c r="F13" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1619.1899999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>44423</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="13">
+        <v>35</v>
+      </c>
+      <c r="F14" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G14" s="16">
+        <v>174.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>44440</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="13">
+        <v>2</v>
+      </c>
+      <c r="F15" s="15">
+        <v>125</v>
+      </c>
+      <c r="G15" s="16">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>44457</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="13">
+        <v>16</v>
+      </c>
+      <c r="F16" s="15">
+        <v>15.99</v>
+      </c>
+      <c r="G16" s="16">
+        <v>255.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>44474</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="13">
+        <v>28</v>
+      </c>
+      <c r="F17" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G17" s="16">
+        <v>251.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>44491</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="13">
+        <v>64</v>
+      </c>
+      <c r="F18" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G18" s="16">
+        <v>575.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>44508</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="13">
+        <v>15</v>
+      </c>
+      <c r="F19" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G19" s="16">
+        <v>299.84999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>44525</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="13">
+        <v>96</v>
+      </c>
+      <c r="F20" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G20" s="16">
+        <v>479.04</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>44542</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="13">
+        <v>67</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G21" s="16">
+        <v>86.43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>44559</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="13">
+        <v>74</v>
+      </c>
+      <c r="F22" s="15">
+        <v>15.99</v>
+      </c>
+      <c r="G22" s="16">
+        <v>1183.26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>44576</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="13">
+        <v>46</v>
+      </c>
+      <c r="F23" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G23" s="16">
+        <v>413.54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>44593</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="13">
+        <v>87</v>
+      </c>
+      <c r="F24" s="15">
+        <v>15</v>
+      </c>
+      <c r="G24" s="16">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>44610</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="13">
+        <v>4</v>
+      </c>
+      <c r="F25" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G25" s="16">
+        <v>19.96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>44627</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="13">
+        <v>7</v>
+      </c>
+      <c r="F26" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G26" s="16">
+        <v>139.92999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>44644</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="13">
+        <v>50</v>
+      </c>
+      <c r="F27" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G27" s="16">
+        <v>249.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
+        <v>44661</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="13">
+        <v>66</v>
+      </c>
+      <c r="F28" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G28" s="16">
+        <v>131.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>44678</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="13">
+        <v>96</v>
+      </c>
+      <c r="F29" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G29" s="16">
+        <v>479.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
+        <v>44695</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="13">
+        <v>53</v>
+      </c>
+      <c r="F30" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G30" s="16">
+        <v>68.37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
+        <v>44712</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="13">
+        <v>80</v>
+      </c>
+      <c r="F31" s="15">
+        <v>8.99</v>
+      </c>
+      <c r="G31" s="16">
+        <v>719.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>44729</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="13">
+        <v>5</v>
+      </c>
+      <c r="F32" s="15">
+        <v>125</v>
+      </c>
+      <c r="G32" s="16">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>44746</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="13">
+        <v>62</v>
+      </c>
+      <c r="F33" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G33" s="16">
+        <v>309.38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
+        <v>44763</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="13">
+        <v>55</v>
+      </c>
+      <c r="F34" s="15">
+        <v>12.49</v>
+      </c>
+      <c r="G34" s="16">
+        <v>686.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>44780</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="13">
+        <v>42</v>
+      </c>
+      <c r="F35" s="15">
+        <v>23.95</v>
+      </c>
+      <c r="G35" s="16">
+        <v>1005.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>44797</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="13">
+        <v>3</v>
+      </c>
+      <c r="F36" s="15">
+        <v>275</v>
+      </c>
+      <c r="G36" s="16">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
+        <v>44814</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="13">
+        <v>7</v>
+      </c>
+      <c r="F37" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G37" s="16">
+        <v>9.0300000000000011</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>44831</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="13">
+        <v>76</v>
+      </c>
+      <c r="F38" s="15">
+        <v>1.99</v>
+      </c>
+      <c r="G38" s="16">
+        <v>151.24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>44848</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="13">
+        <v>57</v>
+      </c>
+      <c r="F39" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G39" s="16">
+        <v>1139.4299999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
+        <v>44865</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="13">
+        <v>14</v>
+      </c>
+      <c r="F40" s="15">
+        <v>1.29</v>
+      </c>
+      <c r="G40" s="16">
+        <v>18.060000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>44882</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="13">
+        <v>11</v>
+      </c>
+      <c r="F41" s="15">
+        <v>4.99</v>
+      </c>
+      <c r="G41" s="16">
+        <v>54.89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="12">
+        <v>44899</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="13">
+        <v>94</v>
+      </c>
+      <c r="F42" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G42" s="16">
+        <v>1879.06</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>44916</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="18">
+        <v>28</v>
+      </c>
+      <c r="F43" s="20">
+        <v>4.99</v>
+      </c>
+      <c r="G43" s="21">
+        <v>139.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <Structure xmlns="thqs">{"Id":"00000000-0000-0000-0000-000000000000","ParentId":null,"Name":"Root","IsExpanded":false,"Children":[]}</Structure>
 </file>

</xml_diff>